<commit_message>
caso de uso modificacion
</commit_message>
<xml_diff>
--- a/casos de uso.xlsx
+++ b/casos de uso.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectoFinalLumaca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5F89C5-4E08-4FEA-BB5F-912E8A59FDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9F3AAB-2773-49F8-AE5E-E8E174AB55B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" xr2:uid="{56C8D8D1-95A8-42F2-B604-9A0B9EAC5F4B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>No. Caso de Prueba</t>
   </si>
@@ -72,9 +72,6 @@
     <t>San José, Uruguay</t>
   </si>
   <si>
-    <t>Version 0.0.0.1</t>
-  </si>
-  <si>
     <t>Alta de Auto</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Redirige al form de editar vehiculo y permite editarlo</t>
   </si>
   <si>
-    <t>BuyCarsUy-Venta de vehiculos</t>
-  </si>
-  <si>
     <t>Consultar sobre vehiculo</t>
   </si>
   <si>
@@ -142,13 +136,31 @@
   </si>
   <si>
     <t>Redirige al mensaje de confirmacion, edita mensaje a "Respuesta censurada"</t>
+  </si>
+  <si>
+    <t>Nombre del proyecto:</t>
+  </si>
+  <si>
+    <t>Navegador:</t>
+  </si>
+  <si>
+    <t>BuyCarsUy</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Version 1.0.0.0</t>
+  </si>
+  <si>
+    <t>BuyCarsUy-Venta y posteo de vehiculos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +176,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -174,18 +194,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -193,19 +213,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,6 +260,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4916EF40-5BD7-4DD5-A2D5-E8C1F4DC4863}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,282 +606,292 @@
     <col min="6" max="6" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>45457</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45459</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3">
         <v>45459</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3">
         <v>45459</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45460</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45460</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45461</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45459</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45462</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45460</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>6</v>
-      </c>
-      <c r="B11" s="6">
-        <v>45460</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45462</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45461</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45463</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>8</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45462</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>9</v>
-      </c>
-      <c r="B14" s="6">
-        <v>45462</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>10</v>
-      </c>
-      <c r="B15" s="6">
-        <v>45463</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B1:C1"/>
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>